<commit_message>
add edited mobile testing checklist
</commit_message>
<xml_diff>
--- a/checklist mobile testing.xlsx
+++ b/checklist mobile testing.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="130">
   <si>
     <t>Чек-лист проверок мобильного приложения</t>
   </si>
@@ -100,6 +100,114 @@
     <t>смена соединения с одного мобильного оператора на другой</t>
   </si>
   <si>
+    <t>смена ориентации с вертикального на горизонтальный</t>
+  </si>
+  <si>
+    <t>смена ориентации</t>
+  </si>
+  <si>
+    <t>интерфейс мобильного приложения адаптируется к экрану устройства</t>
+  </si>
+  <si>
+    <t>запуск приложения в горизонтальной ориентации и смена на вертикальный</t>
+  </si>
+  <si>
+    <t>смена ориентации на на 90 вправо и потом резкое поворачивание на 180 влево</t>
+  </si>
+  <si>
+    <t>смена ориентации на на 90 влево и потом резкое поворачивание на 180 вправо</t>
+  </si>
+  <si>
+    <t>выключение функции смены ориентации на системном уровне и поворачивание экрана в работающем приложении</t>
+  </si>
+  <si>
+    <t>интерфейс мобильного приложения не меняеться</t>
+  </si>
+  <si>
+    <t>смена ориентации с заблокированым экраном</t>
+  </si>
+  <si>
+    <t>интерфейс мобильного приложения адаптируется к экрану устройства после разблокировки</t>
+  </si>
+  <si>
+    <t>минимальный поворот для перехода в горизонтальный режим</t>
+  </si>
+  <si>
+    <t>интерфейс мобильного приложения меняет ориентацию</t>
+  </si>
+  <si>
+    <t>минимальный поворот для перехода в вертикальный  режим</t>
+  </si>
+  <si>
+    <t>быстрое поворачивание экрана в разные стороны</t>
+  </si>
+  <si>
+    <t>интерфейс мобильного приложения меняет ориентацию после остановки поворачивания</t>
+  </si>
+  <si>
+    <t>поворачивание экрана вперед и назад</t>
+  </si>
+  <si>
+    <t>работа через Wi-Fi</t>
+  </si>
+  <si>
+    <t>связь с интернетом</t>
+  </si>
+  <si>
+    <t>работа через 5g</t>
+  </si>
+  <si>
+    <t>работа через 4g</t>
+  </si>
+  <si>
+    <t>работа через 3g</t>
+  </si>
+  <si>
+    <t>работа через 2g</t>
+  </si>
+  <si>
+    <t>тетирование push-уведомлений</t>
+  </si>
+  <si>
+    <t>тестирование pop-up</t>
+  </si>
+  <si>
+    <t>поддержка транзакций через Visa, Mastercard, Paypal</t>
+  </si>
+  <si>
+    <t>темная/светлая темы</t>
+  </si>
+  <si>
+    <t>фильтры</t>
+  </si>
+  <si>
+    <t>шаринг контента в соц.сети</t>
+  </si>
+  <si>
+    <t>реклама в приложении</t>
+  </si>
+  <si>
+    <t>политики конфиденциальности и прочие ссылки на документы</t>
+  </si>
+  <si>
+    <t xml:space="preserve">поля ввода </t>
+  </si>
+  <si>
+    <t>экранная клавиатура появляется сразу после того, как пользователь нажимает на поле ввода, набор без задержек и запинаний</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Тестирование совместимости</t>
+  </si>
+  <si>
+    <t>корректное отображение гео</t>
+  </si>
+  <si>
+    <t>способы оплаты (Google Pay, Apple Pay)</t>
+  </si>
+  <si>
     <t>уведомление о нехватке памяти</t>
   </si>
   <si>
@@ -145,9 +253,18 @@
     <t>перезагрузка телефона</t>
   </si>
   <si>
+    <t xml:space="preserve">сворачивание </t>
+  </si>
+  <si>
+    <t xml:space="preserve">разворачивание </t>
+  </si>
+  <si>
     <t>переключение между приложениями</t>
   </si>
   <si>
+    <t xml:space="preserve">приложение переходит в свернутый режим, после обратного переключения, приложение продолжает работу с последней операции </t>
+  </si>
+  <si>
     <t>push-уведомление</t>
   </si>
   <si>
@@ -172,61 +289,19 @@
     <t>сворачивание в Home</t>
   </si>
   <si>
+    <t>приложение продолжает работу с последней операции после разворачивания</t>
+  </si>
+  <si>
     <t>Screenshot</t>
   </si>
   <si>
+    <t>после снимка экрана приложение продолжае роботу</t>
+  </si>
+  <si>
     <t>регулировка громкости</t>
   </si>
   <si>
-    <t>смена ориентации с вертикального на горизонтальный</t>
-  </si>
-  <si>
-    <t>смена ориентации</t>
-  </si>
-  <si>
-    <t>запуск приложения в горизонтальной ориентации и смена на вертикальный</t>
-  </si>
-  <si>
-    <t>смена ориентации на на 90 вправо и потом резкое поворачивание на 180 влево</t>
-  </si>
-  <si>
-    <t>смена ориентации на на 90 влево и потом резкое поворачивание на 180 вправо</t>
-  </si>
-  <si>
-    <t>выключение функции смены ориентации на системном уровне и поворачивание экрана в работающем приложении</t>
-  </si>
-  <si>
-    <t>смена ориентации с заблокированым экраном</t>
-  </si>
-  <si>
-    <t>минимальный поворот для перехода в горизонтальный режим</t>
-  </si>
-  <si>
-    <t>минимальный поворот для перехода в вертикальный  режим</t>
-  </si>
-  <si>
-    <t>быстрое поворачивание экрана в разные стороны</t>
-  </si>
-  <si>
-    <t>поворачивание экрана вперед и назад</t>
-  </si>
-  <si>
-    <t>II</t>
-  </si>
-  <si>
-    <t>Тестирование совместимости</t>
-  </si>
-  <si>
-    <t>III</t>
-  </si>
-  <si>
-    <t>Тестирование безопасности</t>
-  </si>
-  <si>
-    <t>IV</t>
-  </si>
-  <si>
-    <t>Тестирование локализации и глобализации</t>
+    <t>регулировка громкости не прерывает роботу приложения</t>
   </si>
   <si>
     <t>V</t>
@@ -244,7 +319,7 @@
     <t>значки и изображения выглядят естественно в среде приложения</t>
   </si>
   <si>
-    <t>цвета кнопок, выполняющих ту или иную функцию соответствуют требованиям</t>
+    <t>кнопки, имеющие одинаковую функцию, имеют одинаковый цвет</t>
   </si>
   <si>
     <t>проверка текста на четкость, видимость и простоту восприятия для пользователя</t>
@@ -268,12 +343,36 @@
     <t>обязательные поля отображаются на экране иначе, чем необязательные поля.</t>
   </si>
   <si>
+    <t>приложение предоставляет доступное руководство для пользователей, которые впервые авторизовались</t>
+  </si>
+  <si>
+    <t>увеличения и уменьшения масштаба касанием</t>
+  </si>
+  <si>
     <t>VI</t>
   </si>
   <si>
     <t>Стрессовое тестирование</t>
   </si>
   <si>
+    <t>высокая загрузка центрального процессора</t>
+  </si>
+  <si>
+    <t>нехватка памяти</t>
+  </si>
+  <si>
+    <t>минимальное покрытие сети</t>
+  </si>
+  <si>
+    <t>низкая скорость интернета</t>
+  </si>
+  <si>
+    <t>большое количество взаимодействий пользователя с приложением</t>
+  </si>
+  <si>
+    <t>полный заряд батареи и подключенное зарядное устройство</t>
+  </si>
+  <si>
     <t>VII</t>
   </si>
   <si>
@@ -284,6 +383,24 @@
   </si>
   <si>
     <t>Тестирование производительности</t>
+  </si>
+  <si>
+    <t>время обработки запросов</t>
+  </si>
+  <si>
+    <t>соответствует требованиям</t>
+  </si>
+  <si>
+    <t>потребление заряда батареи</t>
+  </si>
+  <si>
+    <t>потребление оперативной памяти системы</t>
+  </si>
+  <si>
+    <t>время загрузки приложения</t>
+  </si>
+  <si>
+    <t>кэширование данных</t>
   </si>
 </sst>
 </file>
@@ -323,15 +440,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF111111"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10.0"/>
-      <color rgb="FF111111"/>
-      <name val="Arial"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -443,33 +560,33 @@
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="4" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    </xf>
     <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,7 +807,7 @@
     <col customWidth="1" min="1" max="1" width="5.25"/>
     <col customWidth="1" min="2" max="2" width="72.13"/>
     <col customWidth="1" min="3" max="3" width="22.25"/>
-    <col customWidth="1" min="4" max="4" width="44.38"/>
+    <col customWidth="1" min="4" max="4" width="45.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -934,106 +1051,112 @@
         <v>30</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="8"/>
       <c r="B27" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="8"/>
       <c r="B28" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="8"/>
-      <c r="B29" s="7" t="s">
-        <v>38</v>
+      <c r="B29" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>39</v>
+      <c r="D29" s="9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="8"/>
       <c r="B30" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>39</v>
+      <c r="D30" s="9" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="8"/>
       <c r="B31" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="8"/>
       <c r="B32" s="7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="7" t="s">
         <v>30</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="8"/>
       <c r="B33" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="8"/>
       <c r="B34" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>30</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="8"/>
       <c r="B35" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="36">
@@ -1042,7 +1165,7 @@
         <v>47</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37">
@@ -1051,7 +1174,7 @@
         <v>48</v>
       </c>
       <c r="C37" s="7" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="38">
@@ -1060,7 +1183,7 @@
         <v>49</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="39">
@@ -1069,243 +1192,331 @@
         <v>50</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="8"/>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="C40" s="7"/>
     </row>
     <row r="41">
       <c r="A41" s="8"/>
       <c r="B41" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>42</v>
-      </c>
+      <c r="C41" s="7"/>
     </row>
     <row r="42">
       <c r="A42" s="8"/>
       <c r="B42" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="C42" s="7"/>
     </row>
     <row r="43">
       <c r="A43" s="8"/>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="7" t="s">
-        <v>30</v>
-      </c>
+      <c r="C43" s="7"/>
     </row>
     <row r="44">
       <c r="A44" s="8"/>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="C44" s="7"/>
     </row>
     <row r="45">
       <c r="A45" s="8"/>
-      <c r="B45" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C45" s="7" t="s">
+      <c r="B45" s="11" t="s">
         <v>56</v>
       </c>
+      <c r="C45" s="7"/>
     </row>
     <row r="46">
       <c r="A46" s="8"/>
-      <c r="B46" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B46" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C46" s="7"/>
     </row>
     <row r="47">
       <c r="A47" s="8"/>
-      <c r="B47" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B47" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="7"/>
     </row>
     <row r="48">
       <c r="A48" s="8"/>
       <c r="B48" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C48" s="7" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="49">
-      <c r="A49" s="8"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C49" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B49" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="6"/>
     </row>
     <row r="50">
       <c r="A50" s="8"/>
-      <c r="B50" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B50" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="8"/>
     </row>
     <row r="51">
       <c r="A51" s="8"/>
-      <c r="B51" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="B51" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C51" s="8"/>
     </row>
     <row r="52">
       <c r="A52" s="8"/>
       <c r="B52" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="8"/>
       <c r="B53" s="7" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>56</v>
+        <v>66</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B54" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="C54" s="6"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
+      <c r="B55" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
+      <c r="B56" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
+      <c r="B57" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="8"/>
-      <c r="B58" s="8"/>
-      <c r="C58" s="8"/>
+      <c r="B58" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="8"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
+      <c r="A59" s="14"/>
+      <c r="B59" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
+      <c r="B60" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
+      <c r="B61" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
+      <c r="B62" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
+      <c r="B63" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B64" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="C64" s="6"/>
+      <c r="A64" s="8"/>
+      <c r="B64" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
+      <c r="B65" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="8"/>
-      <c r="B66" s="8"/>
-      <c r="C66" s="8"/>
+      <c r="B66" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="8"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
+      <c r="B67" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
+      <c r="B68" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
+      <c r="B69" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
+      <c r="A70" s="14"/>
+      <c r="B70" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
+      <c r="B71" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="8"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
+      <c r="B72" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="8"/>
@@ -1318,13 +1529,9 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75">
-      <c r="A75" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="B75" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="C75" s="6"/>
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
     </row>
     <row r="76">
       <c r="A76" s="8"/>
@@ -1362,192 +1569,367 @@
       <c r="C82" s="8"/>
     </row>
     <row r="83">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
+      <c r="A83" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C83" s="6"/>
     </row>
     <row r="84">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
+      <c r="A84" s="14"/>
+      <c r="B84" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="16"/>
     </row>
     <row r="85">
       <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
+      <c r="B85" s="7" t="s">
+        <v>100</v>
+      </c>
       <c r="C85" s="8"/>
     </row>
     <row r="86">
       <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
+      <c r="B86" s="7" t="s">
+        <v>101</v>
+      </c>
       <c r="C86" s="8"/>
     </row>
     <row r="87">
       <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
+      <c r="B87" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="C87" s="8"/>
     </row>
     <row r="88">
-      <c r="A88" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B88" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" s="6"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" s="8"/>
     </row>
     <row r="89">
-      <c r="A89" s="14"/>
-      <c r="B89" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C89" s="16"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="8"/>
     </row>
     <row r="90">
       <c r="A90" s="8"/>
       <c r="B90" s="7" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C90" s="8"/>
     </row>
     <row r="91">
       <c r="A91" s="8"/>
       <c r="B91" s="7" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
       <c r="C91" s="8"/>
     </row>
     <row r="92">
       <c r="A92" s="8"/>
-      <c r="B92" s="7" t="s">
-        <v>77</v>
+      <c r="B92" s="11" t="s">
+        <v>107</v>
       </c>
       <c r="C92" s="8"/>
     </row>
     <row r="93">
       <c r="A93" s="8"/>
-      <c r="B93" s="7" t="s">
-        <v>78</v>
+      <c r="B93" s="11" t="s">
+        <v>108</v>
       </c>
       <c r="C93" s="8"/>
     </row>
     <row r="94">
       <c r="A94" s="8"/>
-      <c r="B94" s="7" t="s">
-        <v>79</v>
+      <c r="B94" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C94" s="8"/>
     </row>
     <row r="95">
       <c r="A95" s="8"/>
-      <c r="B95" s="7" t="s">
-        <v>80</v>
+      <c r="B95" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="C95" s="8"/>
     </row>
     <row r="96">
       <c r="A96" s="8"/>
-      <c r="B96" s="7" t="s">
-        <v>81</v>
+      <c r="B96" s="11" t="s">
+        <v>111</v>
       </c>
       <c r="C96" s="8"/>
     </row>
     <row r="97">
       <c r="A97" s="8"/>
-      <c r="B97" s="15" t="s">
-        <v>82</v>
-      </c>
+      <c r="B97" s="11"/>
       <c r="C97" s="8"/>
     </row>
     <row r="98">
-      <c r="A98" s="8"/>
-      <c r="B98" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="C98" s="8"/>
+      <c r="A98" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C98" s="6"/>
     </row>
     <row r="99">
-      <c r="A99" s="8"/>
-      <c r="B99" s="15" t="s">
-        <v>84</v>
+      <c r="A99" s="17"/>
+      <c r="B99" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="C99" s="8"/>
     </row>
     <row r="100">
-      <c r="A100" s="8"/>
-      <c r="B100" s="15"/>
+      <c r="A100" s="17"/>
+      <c r="B100" s="11" t="s">
+        <v>115</v>
+      </c>
       <c r="C100" s="8"/>
     </row>
     <row r="101">
-      <c r="A101" s="8"/>
-      <c r="B101" s="15"/>
+      <c r="A101" s="17"/>
+      <c r="B101" s="11" t="s">
+        <v>116</v>
+      </c>
       <c r="C101" s="8"/>
     </row>
     <row r="102">
-      <c r="A102" s="8"/>
-      <c r="B102" s="15"/>
+      <c r="A102" s="17"/>
+      <c r="B102" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="C102" s="8"/>
     </row>
     <row r="103">
-      <c r="A103" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B103" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C103" s="6"/>
+      <c r="A103" s="17"/>
+      <c r="B103" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C103" s="8"/>
     </row>
     <row r="104">
       <c r="A104" s="17"/>
-      <c r="B104" s="18"/>
+      <c r="B104" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="C104" s="8"/>
     </row>
     <row r="105">
-      <c r="A105" s="17"/>
-      <c r="B105" s="18"/>
-      <c r="C105" s="8"/>
+      <c r="A105" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C105" s="6"/>
     </row>
     <row r="106">
-      <c r="A106" s="17"/>
-      <c r="B106" s="18"/>
+      <c r="A106" s="18"/>
+      <c r="B106" s="19"/>
       <c r="C106" s="8"/>
     </row>
     <row r="107">
-      <c r="A107" s="17"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="8"/>
+      <c r="A107" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C107" s="6"/>
     </row>
     <row r="108">
-      <c r="A108" s="17"/>
-      <c r="B108" s="18"/>
-      <c r="C108" s="8"/>
+      <c r="A108" s="8"/>
+      <c r="B108" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="109">
-      <c r="A109" s="17"/>
-      <c r="B109" s="18"/>
-      <c r="C109" s="8"/>
+      <c r="A109" s="8"/>
+      <c r="B109" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="110">
-      <c r="A110" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="C110" s="6"/>
+      <c r="A110" s="8"/>
+      <c r="B110" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C110" s="7"/>
+      <c r="D110" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="111">
-      <c r="A111" s="19"/>
-      <c r="B111" s="18"/>
-      <c r="C111" s="8"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C111" s="7"/>
+      <c r="D111" s="7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="112">
-      <c r="A112" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="B112" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="C112" s="6"/>
+      <c r="A112" s="8"/>
+      <c r="B112" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C112" s="7"/>
+      <c r="D112" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="8"/>
+      <c r="B113" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D113" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="8"/>
+      <c r="B114" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D114" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="8"/>
+      <c r="B115" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D115" s="8"/>
+    </row>
+    <row r="116">
+      <c r="A116" s="8"/>
+      <c r="B116" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D116" s="8"/>
+    </row>
+    <row r="117">
+      <c r="A117" s="8"/>
+      <c r="B117" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="8"/>
+    </row>
+    <row r="118">
+      <c r="A118" s="8"/>
+      <c r="B118" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="8"/>
+    </row>
+    <row r="119">
+      <c r="A119" s="8"/>
+      <c r="B119" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="8"/>
+    </row>
+    <row r="120">
+      <c r="A120" s="8"/>
+      <c r="B120" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="8"/>
+    </row>
+    <row r="121">
+      <c r="A121" s="8"/>
+      <c r="B121" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="8"/>
+    </row>
+    <row r="122">
+      <c r="A122" s="8"/>
+      <c r="B122" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D122" s="8"/>
+    </row>
+    <row r="123">
+      <c r="A123" s="8"/>
+      <c r="B123" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D123" s="8"/>
+    </row>
+    <row r="124">
+      <c r="A124" s="8"/>
+      <c r="B124" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D124" s="8"/>
+    </row>
+    <row r="125">
+      <c r="A125" s="8"/>
+      <c r="B125" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D125" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
add edited checklist mobile testing file
</commit_message>
<xml_diff>
--- a/checklist mobile testing.xlsx
+++ b/checklist mobile testing.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="209">
   <si>
     <t>Чек-лист проверок мобильного приложения</t>
   </si>
@@ -26,6 +26,9 @@
     <t>Expected result</t>
   </si>
   <si>
+    <t>General options</t>
+  </si>
+  <si>
     <t>Функциональное тестирование</t>
   </si>
   <si>
@@ -212,19 +215,64 @@
     <t>работа через 2g</t>
   </si>
   <si>
+    <t>авторизация по номеру телефона</t>
+  </si>
+  <si>
+    <t>приложение успешно авторизирует пользователя</t>
+  </si>
+  <si>
+    <t>авторизация</t>
+  </si>
+  <si>
+    <t>авторизация через соц. сети</t>
+  </si>
+  <si>
+    <t>авторизация через e-mail</t>
+  </si>
+  <si>
+    <t>регистрация по номеру телефона</t>
+  </si>
+  <si>
+    <t>приложение успешно регистрирует пользователя</t>
+  </si>
+  <si>
+    <t>регистрация</t>
+  </si>
+  <si>
+    <t>регистрация через соц. сети</t>
+  </si>
+  <si>
+    <t>регистрация через e-mail</t>
+  </si>
+  <si>
+    <t>валидация обязательных полей</t>
+  </si>
+  <si>
+    <t>успешно валидируються</t>
+  </si>
+  <si>
+    <t xml:space="preserve">редактирование данных </t>
+  </si>
+  <si>
+    <t>возможно редактировать данные в профиле пользователя</t>
+  </si>
+  <si>
     <t>тестирование push-уведомлений</t>
   </si>
   <si>
     <t>с приложения отправляються push-уведомления (можно отключить в настройках приложения)</t>
   </si>
   <si>
-    <t>поддержка транзакций через Visa, Mastercard, Paypal</t>
+    <t>поддержка транзакций</t>
+  </si>
+  <si>
+    <t>поддержка через Visa, Mastercard, Paypal</t>
   </si>
   <si>
     <t>шаринг контента в соц.сети</t>
   </si>
   <si>
-    <t>реклама в приложении</t>
+    <t>контент успешно разпостраняеться</t>
   </si>
   <si>
     <t>политики конфиденциальности и прочие ссылки на документы</t>
@@ -600,7 +648,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d.m"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -632,6 +680,10 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="10.0"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
@@ -646,13 +698,13 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
@@ -718,7 +770,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border/>
     <border>
       <left style="thin">
@@ -764,11 +816,22 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -778,9 +841,6 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
@@ -795,50 +855,59 @@
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="6" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="6" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="5" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="5" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="7" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="4" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1085,1294 +1154,1398 @@
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="4" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="6" t="s">
-        <v>4</v>
+      <c r="A3" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="7">
+      <c r="A4" s="6">
         <v>1.0</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="D4" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="7">
+      <c r="A5" s="6">
         <v>2.0</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="6">
-      <c r="A6" s="7">
+      <c r="A6" s="6">
         <v>3.0</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>7</v>
+      <c r="C6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="7">
+      <c r="A7" s="6">
         <v>4.0</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>7</v>
+      <c r="C7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="7">
+      <c r="A8" s="6">
         <v>5.0</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>7</v>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="7">
+      <c r="A9" s="6">
         <v>6.0</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>7</v>
+      <c r="C9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>7.0</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>7</v>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="7">
+      <c r="A11" s="6">
         <v>8.0</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="8" t="s">
         <v>21</v>
       </c>
+      <c r="D11" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="7">
+      <c r="A12" s="6">
         <v>9.0</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="13">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>10.0</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>21</v>
+      <c r="C13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="7">
+      <c r="A14" s="6">
         <v>11.0</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="6">
+        <v>12.0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="6">
+        <v>13.0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="7">
-        <v>12.0</v>
-      </c>
-      <c r="B15" s="8" t="s">
+      <c r="D16" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="6">
+        <v>14.0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="7">
-        <v>13.0</v>
-      </c>
-      <c r="B16" s="8" t="s">
+      <c r="D17" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="6">
+        <v>15.0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="7">
-        <v>14.0</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="7">
-        <v>15.0</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="7">
-        <v>16.0</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>21</v>
+      <c r="D19" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="7">
+      <c r="A20" s="6">
         <v>17.0</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>21</v>
+      <c r="C20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="7">
+      <c r="A21" s="6">
         <v>18.0</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="8" t="s">
-        <v>21</v>
+      <c r="C21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="7">
+      <c r="A22" s="6">
         <v>19.0</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="9" t="s">
+      <c r="B22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="D22" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="7">
+      <c r="A23" s="6">
         <v>20.0</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="24">
-      <c r="A24" s="7">
+      <c r="A24" s="6">
         <v>21.0</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>45</v>
       </c>
+      <c r="D24" s="7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="7">
+      <c r="A25" s="6">
         <v>22.0</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="8" t="s">
+    </row>
+    <row r="26">
+      <c r="A26" s="6">
+        <v>23.0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="7">
-        <v>23.0</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="7">
-        <v>24.0</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>45</v>
+      <c r="D27" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="7">
+      <c r="A28" s="6">
         <v>25.0</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="B28" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>45</v>
+      <c r="C28" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="7">
+      <c r="A29" s="6">
         <v>26.0</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="B29" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="8" t="s">
-        <v>45</v>
+      <c r="C29" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="7">
+      <c r="A30" s="6">
         <v>27.0</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C30" s="9" t="s">
+      <c r="B30" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D30" s="8" t="s">
-        <v>45</v>
+      <c r="C30" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="7">
+      <c r="A31" s="6">
         <v>28.0</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>45</v>
+      <c r="D31" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="7">
+      <c r="A32" s="6">
         <v>29.0</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="9" t="s">
+      <c r="B32" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>45</v>
+      <c r="C32" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="7">
+      <c r="A33" s="6">
         <v>30.0</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>45</v>
+      <c r="B33" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="7">
+      <c r="A34" s="6">
         <v>31.0</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="D34" s="7" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="7">
+      <c r="A35" s="6">
         <v>32.0</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="8" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" s="6">
+        <v>33.0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="7">
-        <v>33.0</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="8" t="s">
+      <c r="D36" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="6">
+        <v>34.0</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="7">
-        <v>34.0</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="8" t="s">
+      <c r="D37" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="6">
+        <v>35.0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="7" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="7">
-        <v>35.0</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>61</v>
+      <c r="D38" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="7">
+      <c r="A39" s="6">
         <v>36.0</v>
       </c>
-      <c r="B39" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D39" s="8"/>
+      <c r="C39" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="7">
+      <c r="A40" s="6">
         <v>37.0</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="B40" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C40" s="10"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="7">
+      <c r="A41" s="6">
         <v>38.0</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="8"/>
     </row>
     <row r="42">
-      <c r="A42" s="7">
+      <c r="A42" s="6">
         <v>39.0</v>
       </c>
-      <c r="B42" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="8"/>
+      <c r="B42" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="7">
+      <c r="A43" s="6">
         <v>40.0</v>
       </c>
-      <c r="B43" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" s="8"/>
+      <c r="B43" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="7">
+      <c r="A44" s="6">
         <v>41.0</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="D44" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D44" s="8"/>
     </row>
     <row r="45">
-      <c r="A45" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
+      <c r="A45" s="6">
+        <v>42.0</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D45" s="7"/>
     </row>
     <row r="46">
-      <c r="A46" s="7">
-        <v>42.0</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="10"/>
+      <c r="A46" s="6">
+        <v>43.0</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="7"/>
     </row>
     <row r="47">
-      <c r="A47" s="7">
-        <v>43.0</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D47" s="10"/>
+      <c r="A47" s="6">
+        <v>44.0</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" s="7"/>
     </row>
     <row r="48">
-      <c r="A48" s="7">
-        <v>44.0</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A48" s="6">
+        <v>45.0</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D48" s="7"/>
     </row>
     <row r="49">
-      <c r="A49" s="7">
-        <v>45.0</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="C49" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A49" s="6">
+        <v>46.0</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D49" s="7"/>
     </row>
     <row r="50">
-      <c r="A50" s="7">
-        <v>46.0</v>
-      </c>
-      <c r="B50" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A50" s="6">
+        <v>47.0</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="7"/>
     </row>
     <row r="51">
-      <c r="A51" s="7">
-        <v>47.0</v>
-      </c>
-      <c r="B51" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C51" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A51" s="6">
+        <v>48.0</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="D51" s="7"/>
     </row>
     <row r="52">
-      <c r="A52" s="7">
-        <v>48.0</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="A52" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53">
-      <c r="A53" s="7">
+      <c r="A53" s="6">
         <v>49.0</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B53" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D53" s="12"/>
     </row>
     <row r="54">
-      <c r="A54" s="7">
+      <c r="A54" s="6">
         <v>50.0</v>
       </c>
-      <c r="B54" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>21</v>
-      </c>
+      <c r="B54" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D54" s="12"/>
     </row>
     <row r="55">
-      <c r="A55" s="7">
+      <c r="A55" s="6">
         <v>51.0</v>
       </c>
-      <c r="B55" s="8" t="s">
-        <v>91</v>
+      <c r="B55" s="7" t="s">
+        <v>96</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>21</v>
+        <v>97</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="6">
+        <v>52.0</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="13">
-        <v>52.0</v>
-      </c>
-      <c r="B57" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D57" s="10"/>
+      <c r="A57" s="6">
+        <v>53.0</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="7">
-        <v>53.0</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="C58" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D58" s="10"/>
+      <c r="A58" s="14">
+        <v>54.0</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="7">
-        <v>54.0</v>
-      </c>
-      <c r="B59" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D59" s="10"/>
+      <c r="A59" s="6">
+        <v>55.0</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="7">
-        <v>55.0</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D60" s="10"/>
+      <c r="A60" s="6">
+        <v>56.0</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="7">
-        <v>56.0</v>
-      </c>
-      <c r="B61" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="D61" s="10"/>
+      <c r="A61" s="6">
+        <v>57.0</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="7">
-        <v>57.0</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="D62" s="10"/>
+      <c r="A62" s="6">
+        <v>58.0</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="7">
-        <v>58.0</v>
-      </c>
-      <c r="B63" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D63" s="10"/>
+      <c r="A63" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64">
-      <c r="A64" s="7">
+      <c r="A64" s="6">
         <v>59.0</v>
       </c>
-      <c r="B64" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="C64" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D64" s="10"/>
+      <c r="B64" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="D64" s="12"/>
     </row>
     <row r="65">
-      <c r="A65" s="7">
+      <c r="A65" s="6">
         <v>60.0</v>
       </c>
-      <c r="B65" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D65" s="10"/>
+      <c r="B65" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="D65" s="12"/>
     </row>
     <row r="66">
-      <c r="A66" s="7">
+      <c r="A66" s="6">
         <v>61.0</v>
       </c>
-      <c r="B66" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="10"/>
+      <c r="B66" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="D66" s="12"/>
     </row>
     <row r="67">
-      <c r="A67" s="7">
+      <c r="A67" s="6">
         <v>62.0</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>115</v>
-      </c>
-      <c r="D67" s="10"/>
+      <c r="B67" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67" s="12"/>
     </row>
     <row r="68">
-      <c r="A68" s="7">
+      <c r="A68" s="6">
         <v>63.0</v>
       </c>
-      <c r="B68" s="19" t="s">
-        <v>116</v>
+      <c r="B68" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D68" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="D68" s="12"/>
     </row>
     <row r="69">
-      <c r="A69" s="7">
+      <c r="A69" s="6">
         <v>64.0</v>
       </c>
-      <c r="B69" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C69" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="D69" s="10"/>
+      <c r="B69" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D69" s="12"/>
     </row>
     <row r="70">
-      <c r="A70" s="7">
+      <c r="A70" s="6">
         <v>65.0</v>
       </c>
-      <c r="B70" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C70" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D70" s="10"/>
+      <c r="B70" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="D70" s="12"/>
     </row>
     <row r="71">
-      <c r="A71" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
+      <c r="A71" s="6">
+        <v>66.0</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C71" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="D71" s="12"/>
     </row>
     <row r="72">
-      <c r="A72" s="20">
-        <v>66.0</v>
-      </c>
-      <c r="B72" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D72" s="10"/>
+      <c r="A72" s="6">
+        <v>67.0</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" s="12"/>
     </row>
     <row r="73">
-      <c r="A73" s="20">
-        <v>67.0</v>
-      </c>
-      <c r="B73" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D73" s="10"/>
+      <c r="A73" s="19">
+        <v>68.0</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D73" s="12"/>
     </row>
     <row r="74">
-      <c r="A74" s="20">
-        <v>68.0</v>
+      <c r="A74" s="19">
+        <v>69.0</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D74" s="10"/>
+        <v>130</v>
+      </c>
+      <c r="C74" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D74" s="12"/>
     </row>
     <row r="75">
-      <c r="A75" s="20">
-        <v>69.0</v>
-      </c>
-      <c r="B75" s="11" t="s">
-        <v>127</v>
+      <c r="A75" s="19">
+        <v>70.0</v>
+      </c>
+      <c r="B75" s="20" t="s">
+        <v>132</v>
       </c>
       <c r="C75" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D75" s="10"/>
+        <v>133</v>
+      </c>
+      <c r="D75" s="12"/>
     </row>
     <row r="76">
-      <c r="A76" s="20">
-        <v>70.0</v>
+      <c r="A76" s="19">
+        <v>71.0</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D76" s="10"/>
+        <v>134</v>
+      </c>
+      <c r="C76" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="D76" s="12"/>
     </row>
     <row r="77">
-      <c r="A77" s="20">
-        <v>71.0</v>
+      <c r="A77" s="19">
+        <v>72.0</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D77" s="10"/>
+        <v>136</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D77" s="12"/>
     </row>
     <row r="78">
-      <c r="A78" s="6" t="s">
-        <v>130</v>
+      <c r="A78" s="5" t="s">
+        <v>138</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
       <c r="D78" s="3"/>
     </row>
     <row r="79">
-      <c r="A79" s="20">
-        <v>72.0</v>
+      <c r="A79" s="19">
+        <v>73.0</v>
       </c>
       <c r="B79" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
+        <v>139</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D79" s="12"/>
     </row>
     <row r="80">
-      <c r="A80" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
+      <c r="A80" s="19">
+        <v>74.0</v>
+      </c>
+      <c r="B80" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D80" s="12"/>
     </row>
     <row r="81">
-      <c r="A81" s="7">
-        <v>73.0</v>
+      <c r="A81" s="6">
+        <v>75.0</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D81" s="8"/>
+        <v>142</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D81" s="12"/>
     </row>
     <row r="82">
-      <c r="A82" s="7">
-        <v>74.0</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D82" s="8"/>
+      <c r="A82" s="6">
+        <v>76.0</v>
+      </c>
+      <c r="B82" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D82" s="12"/>
     </row>
     <row r="83">
-      <c r="A83" s="7">
-        <v>75.0</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D83" s="8"/>
+      <c r="A83" s="6">
+        <v>77.0</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D83" s="12"/>
     </row>
     <row r="84">
-      <c r="A84" s="7">
-        <v>76.0</v>
+      <c r="A84" s="6">
+        <v>78.0</v>
       </c>
       <c r="B84" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D84" s="8"/>
+        <v>145</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D84" s="12"/>
     </row>
     <row r="85">
-      <c r="A85" s="7">
-        <v>77.0</v>
-      </c>
-      <c r="B85" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D85" s="8"/>
+      <c r="A85" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86">
-      <c r="A86" s="7">
-        <v>78.0</v>
-      </c>
-      <c r="B86" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C86" s="9" t="s">
+      <c r="A86" s="6">
+        <v>79.0</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="C86" s="12"/>
+      <c r="D86" s="12"/>
+    </row>
+    <row r="87">
+      <c r="A87" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B87" s="2"/>
+      <c r="C87" s="2"/>
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88">
+      <c r="A88" s="21">
+        <v>80.0</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D88" s="7"/>
+    </row>
+    <row r="89">
+      <c r="A89" s="22">
+        <v>81.0</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D89" s="7"/>
+    </row>
+    <row r="90">
+      <c r="A90" s="22">
+        <v>82.0</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D90" s="7"/>
+    </row>
+    <row r="91">
+      <c r="A91" s="22">
+        <v>83.0</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D91" s="7"/>
+    </row>
+    <row r="92">
+      <c r="A92" s="22">
+        <v>84.0</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D92" s="7"/>
+    </row>
+    <row r="93">
+      <c r="A93" s="22">
+        <v>85.0</v>
+      </c>
+      <c r="B93" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D86" s="8" t="s">
+      <c r="C93" s="8" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="87">
-      <c r="A87" s="7">
-        <v>79.0</v>
-      </c>
-      <c r="B87" s="8" t="s">
+      <c r="D93" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C87" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D87" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" s="7">
-        <v>80.0</v>
-      </c>
-      <c r="B88" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D88" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" s="7">
-        <v>81.0</v>
-      </c>
-      <c r="B89" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D89" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" s="7">
-        <v>82.0</v>
-      </c>
-      <c r="B90" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D90" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" s="7">
-        <v>83.0</v>
-      </c>
-      <c r="B91" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D91" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" s="7">
-        <v>84.0</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>143</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" s="7">
-        <v>85.0</v>
-      </c>
-      <c r="B93" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D93" s="8" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="94">
-      <c r="A94" s="7">
+      <c r="A94" s="22">
         <v>86.0</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>145</v>
+      <c r="B94" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>41</v>
+        <v>30</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="7">
+      <c r="A95" s="22">
         <v>87.0</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D95" s="8" t="s">
-        <v>41</v>
+      <c r="B95" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="7">
+      <c r="A96" s="22">
         <v>88.0</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D96" s="8" t="s">
-        <v>41</v>
+      <c r="B96" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="7">
+      <c r="A97" s="22">
         <v>89.0</v>
       </c>
-      <c r="B97" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D97" s="8" t="s">
-        <v>41</v>
+      <c r="B97" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="7">
+      <c r="A98" s="22">
         <v>90.0</v>
       </c>
-      <c r="B98" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="D98" s="8" t="s">
-        <v>41</v>
+      <c r="B98" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="6" t="s">
+      <c r="A99" s="22">
+        <v>91.0</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C99" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="3"/>
+      <c r="D99" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="7">
-        <v>91.0</v>
-      </c>
-      <c r="B100" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D100" s="10"/>
+      <c r="A100" s="22">
+        <v>92.0</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="7">
-        <v>92.0</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>153</v>
-      </c>
-      <c r="C101" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="D101" s="10"/>
+      <c r="A101" s="21">
+        <v>93.0</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="102">
-      <c r="A102" s="7">
-        <v>93.0</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>155</v>
-      </c>
-      <c r="C102" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D102" s="10"/>
+      <c r="A102" s="22">
+        <v>94.0</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="22">
+        <v>95.0</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="6">
+        <v>96.0</v>
+      </c>
+      <c r="B104" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="6">
+        <v>97.0</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B106" s="2"/>
+      <c r="C106" s="2"/>
+      <c r="D106" s="3"/>
+    </row>
+    <row r="107">
+      <c r="A107" s="6">
+        <v>98.0</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>167</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="D107" s="12"/>
+    </row>
+    <row r="108">
+      <c r="A108" s="6">
+        <v>99.0</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D108" s="12"/>
+    </row>
+    <row r="109">
+      <c r="A109" s="6">
+        <v>100.0</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="D109" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A52:D52"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="A78:D78"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A106:D106"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A71:D71"/>
-    <mergeCell ref="A78:D78"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A99:D99"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2393,292 +2566,304 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>157</v>
+      <c r="B1" s="23" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="22">
+      <c r="A2" s="24">
         <v>1.0</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>158</v>
+      <c r="B2" s="25" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="24">
+      <c r="A3" s="26">
         <v>44562.0</v>
       </c>
-      <c r="B3" s="9" t="s">
-        <v>159</v>
+      <c r="B3" s="8" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="24">
+      <c r="A4" s="26">
         <v>44593.0</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>160</v>
+      <c r="B4" s="8" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="24">
+      <c r="A5" s="26">
         <v>44621.0</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>161</v>
+      <c r="B5" s="8" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="24">
+      <c r="A6" s="26">
         <v>44652.0</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>162</v>
+      <c r="B6" s="8" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="24">
+      <c r="A7" s="26">
         <v>44682.0</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>163</v>
+      <c r="B7" s="7" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="24">
+      <c r="A8" s="26">
         <v>44713.0</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>164</v>
+      <c r="B8" s="8" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="24">
+      <c r="A9" s="26">
         <v>44743.0</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>165</v>
+      <c r="B9" s="7" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="22">
+      <c r="A10" s="24">
         <v>2.0</v>
       </c>
-      <c r="B10" s="23" t="s">
-        <v>166</v>
+      <c r="B10" s="25" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="24">
+      <c r="A11" s="26">
         <v>44563.0</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>167</v>
+      <c r="B11" s="7" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="24">
+      <c r="A12" s="26">
         <v>44594.0</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>168</v>
+      <c r="B12" s="7" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="24">
+      <c r="A13" s="26">
         <v>44622.0</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>169</v>
+      <c r="B13" s="8" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="24">
+      <c r="A14" s="26">
         <v>44653.0</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>170</v>
+      <c r="B14" s="7" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="24">
+      <c r="A15" s="26">
         <v>44683.0</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>171</v>
+      <c r="B15" s="8" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="24">
+      <c r="A16" s="26">
         <v>44714.0</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>172</v>
+      <c r="B16" s="7" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="24">
+      <c r="A17" s="26">
         <v>44744.0</v>
       </c>
-      <c r="B17" s="8" t="s">
-        <v>173</v>
+      <c r="B17" s="7" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="24">
+      <c r="A18" s="26">
         <v>44775.0</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>174</v>
+      <c r="B18" s="7" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="24">
+      <c r="A19" s="26">
         <v>44806.0</v>
       </c>
-      <c r="B19" s="8" t="s">
-        <v>175</v>
+      <c r="B19" s="7" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="22">
+      <c r="A20" s="24">
         <v>3.0</v>
       </c>
-      <c r="B20" s="23" t="s">
-        <v>176</v>
+      <c r="B20" s="25" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="24">
+      <c r="A21" s="26">
         <v>44564.0</v>
       </c>
-      <c r="B21" s="8" t="s">
-        <v>177</v>
+      <c r="B21" s="7" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="24">
+      <c r="A22" s="26">
         <v>44595.0</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>178</v>
+      <c r="B22" s="8" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="24">
+      <c r="A23" s="26">
         <v>44623.0</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>179</v>
+      <c r="B23" s="8" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="24">
+      <c r="A24" s="26">
         <v>44654.0</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>180</v>
+      <c r="B24" s="8" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="24">
+      <c r="A25" s="26">
         <v>44684.0</v>
       </c>
-      <c r="B25" s="8" t="s">
-        <v>181</v>
+      <c r="B25" s="7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="22">
+      <c r="A26" s="24">
         <v>4.0</v>
       </c>
-      <c r="B26" s="23" t="s">
-        <v>182</v>
+      <c r="B26" s="25" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="24">
+      <c r="A27" s="26">
         <v>44565.0</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>183</v>
+      <c r="B27" s="7" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="24">
+      <c r="A28" s="26">
         <v>44596.0</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>184</v>
+      <c r="B28" s="8" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="24">
+      <c r="A29" s="26">
         <v>44624.0</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>185</v>
+      <c r="B29" s="8" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="24">
+      <c r="A30" s="26">
         <v>44655.0</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>186</v>
+      <c r="B30" s="8" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="22">
+      <c r="A31" s="24">
         <v>5.0</v>
       </c>
-      <c r="B31" s="25" t="s">
-        <v>187</v>
+      <c r="B31" s="27" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="24">
+      <c r="A32" s="26">
         <v>44566.0</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>188</v>
+      <c r="B32" s="7" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="24">
+      <c r="A33" s="26">
         <v>44597.0</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>189</v>
+      <c r="B33" s="7" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="24">
+      <c r="A34" s="26">
         <v>44625.0</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>190</v>
+      <c r="B34" s="7" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="24">
+      <c r="A35" s="26">
         <v>44656.0</v>
       </c>
-      <c r="B35" s="9" t="s">
-        <v>191</v>
+      <c r="B35" s="8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="24">
+      <c r="A36" s="26">
         <v>44686.0</v>
       </c>
-      <c r="B36" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="B36" s="8" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>